<commit_message>
smarter data provider in utils
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21255" windowHeight="7830"/>
+    <workbookView windowWidth="21255" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
   <si>
     <t>firstName</t>
   </si>
@@ -36,16 +37,28 @@
   <si>
     <t>Customer added successfully</t>
   </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>benny refaelov</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -70,11 +83,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -88,15 +107,61 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,15 +169,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,60 +190,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,6 +205,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -209,181 +222,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,39 +413,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -447,6 +427,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,6 +466,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -492,11 +499,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,145 +518,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -975,7 +988,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1013,4 +1026,37 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added skip testing logic, awesome
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
   <si>
     <t>firstName</t>
   </si>
@@ -66,6 +67,27 @@
   </si>
   <si>
     <t>Rupee</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
   </si>
 </sst>
 </file>
@@ -73,10 +95,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -84,13 +106,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -102,11 +117,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -126,6 +164,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -133,21 +222,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,29 +238,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -185,47 +247,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,19 +262,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,163 +418,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -431,15 +453,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -454,6 +467,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,17 +495,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,20 +519,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,153 +544,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1006,7 +1028,7 @@
   <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1119,4 +1141,53 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
smarter data with table
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>alerttest</t>
+    <t>alerttext</t>
   </si>
   <si>
     <t>runmode</t>
@@ -98,10 +98,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -113,6 +113,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -120,24 +127,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -158,7 +150,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,74 +172,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -248,9 +180,77 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,55 +265,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,127 +445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,11 +459,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,32 +513,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -542,17 +537,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,15 +561,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -579,130 +579,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>

</xml_diff>